<commit_message>
Added Email Address for SubmitPPIPayment for Upgrade and Production Test Data
</commit_message>
<xml_diff>
--- a/FullRefundDataUpgrade.xlsx
+++ b/FullRefundDataUpgrade.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SoapData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD5F550-F708-431E-8265-B21E0C0A588A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20355" windowHeight="13170"/>
+    <workbookView xWindow="1270" yWindow="2430" windowWidth="31880" windowHeight="14900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SaleUpgrade" sheetId="2" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="108">
   <si>
     <t>Notes</t>
   </si>
@@ -345,12 +346,15 @@
   </si>
   <si>
     <t>50018</t>
+  </si>
+  <si>
+    <t>iahmed@govolution.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -395,9 +399,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,90 +682,90 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BW5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BH1" workbookViewId="0">
-      <selection activeCell="BS7" sqref="BS7"/>
+    <sheetView tabSelected="1" topLeftCell="AY1" workbookViewId="0">
+      <selection activeCell="BD2" sqref="BD2:BD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.3828125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.3828125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.53515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.3046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.53515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.3828125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.15234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.3046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.3046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.3046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.3046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.3046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.3046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.15234375" style="1" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="9.140625" style="1"/>
-    <col min="41" max="41" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.3046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="5.3828125" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9.15234375" style="1"/>
+    <col min="41" max="41" width="8.84375" style="1" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.15234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.53515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="10.3828125" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="17.3046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="15.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="19.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="6.3046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.15234375" style="1" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="12.3046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="11.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="5.3828125" style="1" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="34.23046875" style="1" customWidth="1"/>
     <col min="57" max="57" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="16.3046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="12.3046875" style="1" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="14.84375" style="1" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="11.69140625" style="1" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="73" max="16384" width="9.140625" style="1"/>
+    <col min="66" max="66" width="10.53515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="17.53515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="14.15234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="12.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="11.15234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="24.3828125" style="1" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="7.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="73" max="16384" width="9.15234375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:75" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -987,7 +992,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:75" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>79</v>
       </c>
@@ -1039,6 +1044,9 @@
       <c r="BB2" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="BD2" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="BE2" s="1" t="s">
         <v>101</v>
       </c>
@@ -1076,7 +1084,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:75" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>91</v>
       </c>
@@ -1128,6 +1136,9 @@
       <c r="BB3" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="BD3" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="BE3" s="1" t="s">
         <v>101</v>
       </c>
@@ -1168,7 +1179,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:75" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>92</v>
       </c>
@@ -1220,6 +1231,9 @@
       <c r="BB4" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="BD4" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="BE4" s="1" t="s">
         <v>101</v>
       </c>
@@ -1260,7 +1274,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:75" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>93</v>
       </c>
@@ -1305,6 +1319,9 @@
       </c>
       <c r="AW5" s="1" t="s">
         <v>75</v>
+      </c>
+      <c r="BD5" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="BE5" s="1" t="s">
         <v>101</v>
@@ -1355,5 +1372,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>